<commit_message>
update bẳng phân công công việc
</commit_message>
<xml_diff>
--- a/Bảng phân công công việc.xlsx
+++ b/Bảng phân công công việc.xlsx
@@ -121,9 +121,6 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -139,6 +136,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -448,80 +448,80 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="32.42578125" customWidth="1"/>
     <col min="3" max="3" width="45.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1"/>
-      <c r="D1" s="6"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="8">
-        <v>0.7</v>
+      <c r="D4" s="7">
+        <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="8">
-        <v>0.1</v>
+      <c r="D5" s="7">
+        <v>0.2</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="8">
-        <v>0.1</v>
+      <c r="D6" s="7">
+        <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="8">
-        <v>0.1</v>
+      <c r="D7" s="7">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>